<commit_message>
Add Figure describing contributions by region and study
</commit_message>
<xml_diff>
--- a/2_Methane_Database/Table_Comp_Emissions.xlsx
+++ b/2_Methane_Database/Table_Comp_Emissions.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ru3\Dropbox\Doctoral\Projects\Research Projects\manuscripts\2_BU_paper\3_Analysis\2_Methane_Database\FINAL POST REVISION VERSIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264B382C-FC7C-4592-85BB-3581CCD99F75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E81A12-EBD9-42F4-93C4-63B6D38378DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="16440" xr2:uid="{F1F3538F-0AEA-4C20-8170-01D92509DDFA}"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{F1F3538F-0AEA-4C20-8170-01D92509DDFA}"/>
   </bookViews>
   <sheets>
     <sheet name="EF_Study" sheetId="2" r:id="rId1"/>
     <sheet name="EF_Component" sheetId="1" r:id="rId2"/>
     <sheet name="EF_Study_Expanded" sheetId="4" r:id="rId3"/>
+    <sheet name="Reg_Distribution" sheetId="5" r:id="rId4"/>
+    <sheet name="Chart2" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="87">
   <si>
     <t>Component</t>
   </si>
@@ -284,6 +286,27 @@
   <si>
     <t>API 19943</t>
   </si>
+  <si>
+    <t>Equipment leaks</t>
+  </si>
+  <si>
+    <t>Tanks</t>
+  </si>
+  <si>
+    <t>Liquids unloadings</t>
+  </si>
+  <si>
+    <t>TC/F</t>
+  </si>
+  <si>
+    <t>Hatch/hole/PRV</t>
+  </si>
+  <si>
+    <t>Allen2014b</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
 </sst>
 </file>
 
@@ -458,7 +481,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -625,6 +648,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -634,14 +663,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -659,6 +686,1710 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.2828321285453768E-2"/>
+          <c:y val="1.8703978676919059E-2"/>
+          <c:w val="0.89572513794025088"/>
+          <c:h val="0.59763821946499107"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reg_Distribution!$D$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API 1993</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="009B76"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Reg_Distribution!$B$39:$C$53</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="14"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>TC/F</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>VL</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>OEL</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>PRV</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>REG</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Other</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>LU</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Equipment leaks</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Liquids unloadings</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reg_Distribution!$D$39:$D$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-665D-4440-90FA-AAA83BC99F9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reg_Distribution!$E$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Allen2013</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="8C1515"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Reg_Distribution!$B$39:$C$53</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="14"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>TC/F</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>VL</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>OEL</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>PRV</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>REG</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Other</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>LU</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Equipment leaks</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Liquids unloadings</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reg_Distribution!$E$39:$E$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>305</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-665D-4440-90FA-AAA83BC99F9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reg_Distribution!$F$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Allen2014a</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Reg_Distribution!$B$39:$C$53</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="14"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>TC/F</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>VL</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>OEL</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>PRV</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>REG</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Other</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>LU</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Equipment leaks</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Liquids unloadings</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reg_Distribution!$F$39:$F$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="10">
+                  <c:v>377</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-665D-4440-90FA-AAA83BC99F9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reg_Distribution!$G$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bell2017</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E98300"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Reg_Distribution!$B$39:$C$53</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="14"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>TC/F</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>VL</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>OEL</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>PRV</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>REG</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Other</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>LU</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Equipment leaks</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Liquids unloadings</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reg_Distribution!$G$39:$G$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-665D-4440-90FA-AAA83BC99F9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reg_Distribution!$H$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ERG2011</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="D2C295"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Reg_Distribution!$B$39:$C$53</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="14"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>TC/F</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>VL</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>OEL</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>PRV</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>REG</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Other</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>LU</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Equipment leaks</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Liquids unloadings</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reg_Distribution!$H$39:$H$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>481</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>763</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-665D-4440-90FA-AAA83BC99F9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reg_Distribution!$I$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Thoma 2017</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="53284F"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Reg_Distribution!$B$39:$C$53</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="14"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>TC/F</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>VL</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>OEL</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>PRV</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>REG</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Other</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>LU</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Equipment leaks</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Liquids unloadings</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reg_Distribution!$I$39:$I$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="10">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-665D-4440-90FA-AAA83BC99F9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reg_Distribution!$J$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pasci 2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0098DB"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Reg_Distribution!$B$39:$C$53</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="14"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>TC/F</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>VL</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>OEL</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>PRV</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>REG</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Other</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>LU</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Equipment leaks</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Liquids unloadings</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reg_Distribution!$J$39:$J$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-665D-4440-90FA-AAA83BC99F9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reg_Distribution!$K$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Allen2014b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="175E54"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Reg_Distribution!$B$39:$C$53</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="14"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>TC/F</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>VL</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>OEL</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>PRV</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>REG</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Other</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>LU</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Equipment leaks</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Tanks</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Liquids unloadings</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reg_Distribution!$K$39:$K$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="13">
+                  <c:v>107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-665D-4440-90FA-AAA83BC99F9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="10"/>
+        <c:overlap val="100"/>
+        <c:axId val="742788472"/>
+        <c:axId val="578428096"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="742788472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="578428096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="578428096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Quantified</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> measurement count</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.7130800890955804E-2"/>
+              <c:y val="0.24465125954532085"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="742788472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11672788327929601"/>
+          <c:y val="0.73059275166361792"/>
+          <c:w val="0.10974270495599815"/>
+          <c:h val="0.2553128131710809"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1600">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D8260B37-9AA8-42BC-9399-8576F22E7C01}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="12997405" cy="9440601"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{667D8BFA-2F90-4A4C-AB3E-A94A41A7B4CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -960,8 +2691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7153208-F156-487E-9386-C3BE5B3C409B}">
   <dimension ref="B3:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -2653,24 +4384,24 @@
     <row r="6" spans="2:31" ht="15" customHeight="1">
       <c r="B6" s="40"/>
       <c r="C6" s="41"/>
-      <c r="D6" s="68" t="s">
+      <c r="D6" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="68"/>
-      <c r="Q6" s="68"/>
-      <c r="R6" s="68"/>
-      <c r="S6" s="68"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
+      <c r="S6" s="70"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
@@ -2685,7 +4416,7 @@
       <c r="AE6" s="1"/>
     </row>
     <row r="7" spans="2:31" ht="21" customHeight="1">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="71" t="s">
         <v>63</v>
       </c>
       <c r="C7" s="42" t="s">
@@ -2769,7 +4500,7 @@
       <c r="AE7" s="1"/>
     </row>
     <row r="8" spans="2:31" ht="21" customHeight="1">
-      <c r="B8" s="70"/>
+      <c r="B8" s="72"/>
       <c r="C8" s="44" t="s">
         <v>65</v>
       </c>
@@ -2851,7 +4582,7 @@
       <c r="AE8" s="1"/>
     </row>
     <row r="9" spans="2:31" ht="21" customHeight="1">
-      <c r="B9" s="70"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="44" t="s">
         <v>20</v>
       </c>
@@ -2933,7 +4664,7 @@
       <c r="AE9" s="1"/>
     </row>
     <row r="10" spans="2:31" ht="21" customHeight="1">
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="72" t="s">
         <v>66</v>
       </c>
       <c r="C10" s="44" t="s">
@@ -3017,7 +4748,7 @@
       <c r="AE10" s="1"/>
     </row>
     <row r="11" spans="2:31" ht="21" customHeight="1">
-      <c r="B11" s="70"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="44" t="s">
         <v>65</v>
       </c>
@@ -3183,24 +4914,24 @@
     <row r="13" spans="2:31">
       <c r="B13" s="40"/>
       <c r="C13" s="41"/>
-      <c r="D13" s="68" t="s">
+      <c r="D13" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="68"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="68"/>
-      <c r="O13" s="68"/>
-      <c r="P13" s="68"/>
-      <c r="Q13" s="68"/>
-      <c r="R13" s="68"/>
-      <c r="S13" s="68"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="70"/>
+      <c r="M13" s="70"/>
+      <c r="N13" s="70"/>
+      <c r="O13" s="70"/>
+      <c r="P13" s="70"/>
+      <c r="Q13" s="70"/>
+      <c r="R13" s="70"/>
+      <c r="S13" s="70"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
@@ -3215,7 +4946,7 @@
       <c r="AE13" s="1"/>
     </row>
     <row r="14" spans="2:31" ht="21" customHeight="1">
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="71" t="s">
         <v>63</v>
       </c>
       <c r="C14" s="42" t="s">
@@ -3299,7 +5030,7 @@
       <c r="AE14" s="1"/>
     </row>
     <row r="15" spans="2:31" ht="21" customHeight="1">
-      <c r="B15" s="70"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="44" t="s">
         <v>65</v>
       </c>
@@ -3381,7 +5112,7 @@
       <c r="AE15" s="1"/>
     </row>
     <row r="16" spans="2:31" ht="21" customHeight="1">
-      <c r="B16" s="70"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="44" t="s">
         <v>20</v>
       </c>
@@ -3463,7 +5194,7 @@
       <c r="AE16" s="1"/>
     </row>
     <row r="17" spans="2:31" ht="21" customHeight="1">
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="72" t="s">
         <v>66</v>
       </c>
       <c r="C17" s="44" t="s">
@@ -3547,7 +5278,7 @@
       <c r="AE17" s="1"/>
     </row>
     <row r="18" spans="2:31" ht="21" customHeight="1">
-      <c r="B18" s="70"/>
+      <c r="B18" s="72"/>
       <c r="C18" s="44" t="s">
         <v>65</v>
       </c>
@@ -3713,24 +5444,24 @@
     <row r="20" spans="2:31">
       <c r="B20" s="40"/>
       <c r="C20" s="41"/>
-      <c r="D20" s="68" t="s">
+      <c r="D20" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="68"/>
-      <c r="M20" s="68"/>
-      <c r="N20" s="68"/>
-      <c r="O20" s="68"/>
-      <c r="P20" s="68"/>
-      <c r="Q20" s="68"/>
-      <c r="R20" s="68"/>
-      <c r="S20" s="68"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="70"/>
+      <c r="P20" s="70"/>
+      <c r="Q20" s="70"/>
+      <c r="R20" s="70"/>
+      <c r="S20" s="70"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
@@ -3745,7 +5476,7 @@
       <c r="AE20" s="1"/>
     </row>
     <row r="21" spans="2:31" ht="21" customHeight="1">
-      <c r="B21" s="69" t="s">
+      <c r="B21" s="71" t="s">
         <v>63</v>
       </c>
       <c r="C21" s="42" t="s">
@@ -3829,7 +5560,7 @@
       <c r="AE21" s="1"/>
     </row>
     <row r="22" spans="2:31" ht="21" customHeight="1">
-      <c r="B22" s="70"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="44" t="s">
         <v>65</v>
       </c>
@@ -3911,7 +5642,7 @@
       <c r="AE22" s="1"/>
     </row>
     <row r="23" spans="2:31" ht="21" customHeight="1">
-      <c r="B23" s="70"/>
+      <c r="B23" s="72"/>
       <c r="C23" s="44" t="s">
         <v>20</v>
       </c>
@@ -3993,7 +5724,7 @@
       <c r="AE23" s="1"/>
     </row>
     <row r="24" spans="2:31" ht="21" customHeight="1">
-      <c r="B24" s="71" t="s">
+      <c r="B24" s="68" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="44" t="s">
@@ -4077,7 +5808,7 @@
       <c r="AE24" s="1"/>
     </row>
     <row r="25" spans="2:31" ht="21" customHeight="1">
-      <c r="B25" s="71"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="44" t="s">
         <v>65</v>
       </c>
@@ -4159,7 +5890,7 @@
       <c r="AE25" s="1"/>
     </row>
     <row r="26" spans="2:31" ht="21" customHeight="1">
-      <c r="B26" s="72"/>
+      <c r="B26" s="69"/>
       <c r="C26" s="47" t="s">
         <v>20</v>
       </c>
@@ -4243,24 +5974,24 @@
     <row r="27" spans="2:31">
       <c r="B27" s="38"/>
       <c r="C27" s="49"/>
-      <c r="D27" s="68" t="s">
+      <c r="D27" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
-      <c r="M27" s="68"/>
-      <c r="N27" s="68"/>
-      <c r="O27" s="68"/>
-      <c r="P27" s="68"/>
-      <c r="Q27" s="68"/>
-      <c r="R27" s="68"/>
-      <c r="S27" s="68"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="70"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="70"/>
+      <c r="L27" s="70"/>
+      <c r="M27" s="70"/>
+      <c r="N27" s="70"/>
+      <c r="O27" s="70"/>
+      <c r="P27" s="70"/>
+      <c r="Q27" s="70"/>
+      <c r="R27" s="70"/>
+      <c r="S27" s="70"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
@@ -4275,7 +6006,7 @@
       <c r="AE27" s="1"/>
     </row>
     <row r="28" spans="2:31" ht="21" customHeight="1">
-      <c r="B28" s="69" t="s">
+      <c r="B28" s="71" t="s">
         <v>63</v>
       </c>
       <c r="C28" s="42" t="s">
@@ -4359,7 +6090,7 @@
       <c r="AE28" s="1"/>
     </row>
     <row r="29" spans="2:31" ht="21" customHeight="1">
-      <c r="B29" s="70"/>
+      <c r="B29" s="72"/>
       <c r="C29" s="44" t="s">
         <v>65</v>
       </c>
@@ -4441,7 +6172,7 @@
       <c r="AE29" s="1"/>
     </row>
     <row r="30" spans="2:31" ht="21" customHeight="1">
-      <c r="B30" s="70"/>
+      <c r="B30" s="72"/>
       <c r="C30" s="44" t="s">
         <v>20</v>
       </c>
@@ -4523,7 +6254,7 @@
       <c r="AE30" s="1"/>
     </row>
     <row r="31" spans="2:31" ht="21" customHeight="1">
-      <c r="B31" s="71" t="s">
+      <c r="B31" s="68" t="s">
         <v>66</v>
       </c>
       <c r="C31" s="44" t="s">
@@ -4607,7 +6338,7 @@
       <c r="AE31" s="1"/>
     </row>
     <row r="32" spans="2:31" ht="21" customHeight="1">
-      <c r="B32" s="71"/>
+      <c r="B32" s="68"/>
       <c r="C32" s="44" t="s">
         <v>65</v>
       </c>
@@ -4689,7 +6420,7 @@
       <c r="AE32" s="1"/>
     </row>
     <row r="33" spans="2:31" ht="21" customHeight="1">
-      <c r="B33" s="72"/>
+      <c r="B33" s="69"/>
       <c r="C33" s="47" t="s">
         <v>20</v>
       </c>
@@ -4773,24 +6504,24 @@
     <row r="34" spans="2:31">
       <c r="B34" s="40"/>
       <c r="C34" s="41"/>
-      <c r="D34" s="68" t="s">
+      <c r="D34" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="68"/>
-      <c r="K34" s="68"/>
-      <c r="L34" s="68"/>
-      <c r="M34" s="68"/>
-      <c r="N34" s="68"/>
-      <c r="O34" s="68"/>
-      <c r="P34" s="68"/>
-      <c r="Q34" s="68"/>
-      <c r="R34" s="68"/>
-      <c r="S34" s="68"/>
+      <c r="E34" s="70"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="70"/>
+      <c r="M34" s="70"/>
+      <c r="N34" s="70"/>
+      <c r="O34" s="70"/>
+      <c r="P34" s="70"/>
+      <c r="Q34" s="70"/>
+      <c r="R34" s="70"/>
+      <c r="S34" s="70"/>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
@@ -4805,7 +6536,7 @@
       <c r="AE34" s="1"/>
     </row>
     <row r="35" spans="2:31" ht="22.25" customHeight="1">
-      <c r="B35" s="69" t="s">
+      <c r="B35" s="71" t="s">
         <v>63</v>
       </c>
       <c r="C35" s="42" t="s">
@@ -4889,7 +6620,7 @@
       <c r="AE35" s="1"/>
     </row>
     <row r="36" spans="2:31" ht="22.25" customHeight="1">
-      <c r="B36" s="70"/>
+      <c r="B36" s="72"/>
       <c r="C36" s="44" t="s">
         <v>65</v>
       </c>
@@ -4971,7 +6702,7 @@
       <c r="AE36" s="1"/>
     </row>
     <row r="37" spans="2:31" ht="22.25" customHeight="1">
-      <c r="B37" s="70"/>
+      <c r="B37" s="72"/>
       <c r="C37" s="44" t="s">
         <v>20</v>
       </c>
@@ -5053,7 +6784,7 @@
       <c r="AE37" s="1"/>
     </row>
     <row r="38" spans="2:31" ht="22.25" customHeight="1">
-      <c r="B38" s="71" t="s">
+      <c r="B38" s="68" t="s">
         <v>66</v>
       </c>
       <c r="C38" s="44" t="s">
@@ -5137,7 +6868,7 @@
       <c r="AE38" s="1"/>
     </row>
     <row r="39" spans="2:31" ht="22.25" customHeight="1">
-      <c r="B39" s="71"/>
+      <c r="B39" s="68"/>
       <c r="C39" s="44" t="s">
         <v>65</v>
       </c>
@@ -5219,7 +6950,7 @@
       <c r="AE39" s="1"/>
     </row>
     <row r="40" spans="2:31" ht="22.25" customHeight="1">
-      <c r="B40" s="72"/>
+      <c r="B40" s="69"/>
       <c r="C40" s="47" t="s">
         <v>20</v>
       </c>
@@ -5303,24 +7034,24 @@
     <row r="41" spans="2:31">
       <c r="B41" s="40"/>
       <c r="C41" s="41"/>
-      <c r="D41" s="68" t="s">
+      <c r="D41" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="E41" s="68"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="68"/>
-      <c r="J41" s="68"/>
-      <c r="K41" s="68"/>
-      <c r="L41" s="68"/>
-      <c r="M41" s="68"/>
-      <c r="N41" s="68"/>
-      <c r="O41" s="68"/>
-      <c r="P41" s="68"/>
-      <c r="Q41" s="68"/>
-      <c r="R41" s="68"/>
-      <c r="S41" s="68"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="70"/>
+      <c r="J41" s="70"/>
+      <c r="K41" s="70"/>
+      <c r="L41" s="70"/>
+      <c r="M41" s="70"/>
+      <c r="N41" s="70"/>
+      <c r="O41" s="70"/>
+      <c r="P41" s="70"/>
+      <c r="Q41" s="70"/>
+      <c r="R41" s="70"/>
+      <c r="S41" s="70"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
@@ -5335,7 +7066,7 @@
       <c r="AE41" s="1"/>
     </row>
     <row r="42" spans="2:31" ht="21" customHeight="1">
-      <c r="B42" s="69" t="s">
+      <c r="B42" s="71" t="s">
         <v>63</v>
       </c>
       <c r="C42" s="42" t="s">
@@ -5419,7 +7150,7 @@
       <c r="AE42" s="1"/>
     </row>
     <row r="43" spans="2:31" ht="21" customHeight="1">
-      <c r="B43" s="70"/>
+      <c r="B43" s="72"/>
       <c r="C43" s="44" t="s">
         <v>65</v>
       </c>
@@ -5501,7 +7232,7 @@
       <c r="AE43" s="1"/>
     </row>
     <row r="44" spans="2:31" ht="21" customHeight="1">
-      <c r="B44" s="70"/>
+      <c r="B44" s="72"/>
       <c r="C44" s="44" t="s">
         <v>20</v>
       </c>
@@ -5583,7 +7314,7 @@
       <c r="AE44" s="1"/>
     </row>
     <row r="45" spans="2:31" ht="21" customHeight="1">
-      <c r="B45" s="71" t="s">
+      <c r="B45" s="68" t="s">
         <v>66</v>
       </c>
       <c r="C45" s="44" t="s">
@@ -5667,7 +7398,7 @@
       <c r="AE45" s="1"/>
     </row>
     <row r="46" spans="2:31" ht="21" customHeight="1">
-      <c r="B46" s="71"/>
+      <c r="B46" s="68"/>
       <c r="C46" s="44" t="s">
         <v>65</v>
       </c>
@@ -5749,7 +7480,7 @@
       <c r="AE46" s="1"/>
     </row>
     <row r="47" spans="2:31" ht="21" customHeight="1">
-      <c r="B47" s="72"/>
+      <c r="B47" s="69"/>
       <c r="C47" s="47" t="s">
         <v>20</v>
       </c>
@@ -5833,24 +7564,24 @@
     <row r="48" spans="2:31">
       <c r="B48" s="40"/>
       <c r="C48" s="41"/>
-      <c r="D48" s="68" t="s">
+      <c r="D48" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="E48" s="68"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="68"/>
-      <c r="H48" s="68"/>
-      <c r="I48" s="68"/>
-      <c r="J48" s="68"/>
-      <c r="K48" s="68"/>
-      <c r="L48" s="68"/>
-      <c r="M48" s="68"/>
-      <c r="N48" s="68"/>
-      <c r="O48" s="68"/>
-      <c r="P48" s="68"/>
-      <c r="Q48" s="68"/>
-      <c r="R48" s="68"/>
-      <c r="S48" s="68"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="70"/>
+      <c r="G48" s="70"/>
+      <c r="H48" s="70"/>
+      <c r="I48" s="70"/>
+      <c r="J48" s="70"/>
+      <c r="K48" s="70"/>
+      <c r="L48" s="70"/>
+      <c r="M48" s="70"/>
+      <c r="N48" s="70"/>
+      <c r="O48" s="70"/>
+      <c r="P48" s="70"/>
+      <c r="Q48" s="70"/>
+      <c r="R48" s="70"/>
+      <c r="S48" s="70"/>
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
       <c r="V48" s="1"/>
@@ -5865,7 +7596,7 @@
       <c r="AE48" s="1"/>
     </row>
     <row r="49" spans="2:31" ht="24" customHeight="1">
-      <c r="B49" s="69" t="s">
+      <c r="B49" s="71" t="s">
         <v>63</v>
       </c>
       <c r="C49" s="44" t="s">
@@ -5949,7 +7680,7 @@
       <c r="AE49" s="1"/>
     </row>
     <row r="50" spans="2:31" ht="24" customHeight="1">
-      <c r="B50" s="70"/>
+      <c r="B50" s="72"/>
       <c r="C50" s="44" t="s">
         <v>65</v>
       </c>
@@ -6031,7 +7762,7 @@
       <c r="AE50" s="1"/>
     </row>
     <row r="51" spans="2:31" ht="24" customHeight="1">
-      <c r="B51" s="70"/>
+      <c r="B51" s="72"/>
       <c r="C51" s="44" t="s">
         <v>20</v>
       </c>
@@ -6113,7 +7844,7 @@
       <c r="AE51" s="1"/>
     </row>
     <row r="52" spans="2:31" ht="24" customHeight="1">
-      <c r="B52" s="71" t="s">
+      <c r="B52" s="68" t="s">
         <v>66</v>
       </c>
       <c r="C52" s="44" t="s">
@@ -6197,7 +7928,7 @@
       <c r="AE52" s="1"/>
     </row>
     <row r="53" spans="2:31" ht="24" customHeight="1">
-      <c r="B53" s="71"/>
+      <c r="B53" s="68"/>
       <c r="C53" s="44" t="s">
         <v>65</v>
       </c>
@@ -6279,7 +8010,7 @@
       <c r="AE53" s="1"/>
     </row>
     <row r="54" spans="2:31" ht="24" customHeight="1">
-      <c r="B54" s="72"/>
+      <c r="B54" s="69"/>
       <c r="C54" s="47" t="s">
         <v>20</v>
       </c>
@@ -10519,6 +12250,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D48:S48"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="D34:S34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="D41:S41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="D6:S6"/>
     <mergeCell ref="B7:B9"/>
@@ -10531,17 +12271,904 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="D27:S27"/>
     <mergeCell ref="B28:B30"/>
-    <mergeCell ref="D48:S48"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="D34:S34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="D41:S41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1019FDB8-E67A-4E6D-9287-00623A9D9229}">
+  <dimension ref="B3:K57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43:I44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="3" spans="2:11">
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="74">
+        <f>EF_Study_Expanded!D9</f>
+        <v>38</v>
+      </c>
+      <c r="D5" s="74">
+        <f>EF_Study_Expanded!E9</f>
+        <v>113</v>
+      </c>
+      <c r="E5" s="74">
+        <f>EF_Study_Expanded!F9</f>
+        <v>54</v>
+      </c>
+      <c r="F5" s="74">
+        <f>EF_Study_Expanded!G9</f>
+        <v>10</v>
+      </c>
+      <c r="G5" s="74"/>
+      <c r="I5" s="74" t="str">
+        <f>EF_Study_Expanded!M9</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J5" s="74">
+        <f>EF_Study_Expanded!R9</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="74">
+        <f>EF_Study_Expanded!D16+EF_Study_Expanded!J16</f>
+        <v>50</v>
+      </c>
+      <c r="D6" s="74">
+        <f>EF_Study_Expanded!E16</f>
+        <v>41</v>
+      </c>
+      <c r="E6" s="74">
+        <f>EF_Study_Expanded!F16</f>
+        <v>5</v>
+      </c>
+      <c r="F6" s="74">
+        <f>EF_Study_Expanded!G16</f>
+        <v>3</v>
+      </c>
+      <c r="G6" s="74">
+        <f>EF_Study_Expanded!I16</f>
+        <v>51</v>
+      </c>
+      <c r="I6" s="74">
+        <f>EF_Study_Expanded!M16</f>
+        <v>305</v>
+      </c>
+      <c r="J6" s="74">
+        <f>EF_Study_Expanded!R16</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="74">
+        <f>EF_Study_Expanded!M23</f>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="74">
+        <f>EF_Study_Expanded!D30+EF_Study_Expanded!J30</f>
+        <v>21</v>
+      </c>
+      <c r="D8" s="74">
+        <f>EF_Study_Expanded!E30</f>
+        <v>9</v>
+      </c>
+      <c r="E8" s="74" t="str">
+        <f>EF_Study_Expanded!F30</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="F8" s="74">
+        <f>EF_Study_Expanded!G30</f>
+        <v>14</v>
+      </c>
+      <c r="G8" s="74">
+        <f>EF_Study_Expanded!I30</f>
+        <v>18</v>
+      </c>
+      <c r="I8" s="74">
+        <f>EF_Study_Expanded!M30</f>
+        <v>41</v>
+      </c>
+      <c r="J8" s="74">
+        <f>EF_Study_Expanded!R30</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="74">
+        <f>EF_Study_Expanded!D37+EF_Study_Expanded!J37</f>
+        <v>481</v>
+      </c>
+      <c r="D9" s="74">
+        <f>EF_Study_Expanded!E37</f>
+        <v>139</v>
+      </c>
+      <c r="E9" s="74">
+        <f>EF_Study_Expanded!F37</f>
+        <v>13</v>
+      </c>
+      <c r="F9" s="74" t="str">
+        <f>EF_Study_Expanded!G37</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G9" s="74">
+        <f>EF_Study_Expanded!I37</f>
+        <v>95</v>
+      </c>
+      <c r="H9" s="74">
+        <f>EF_Study_Expanded!O37+EF_Study_Expanded!P37</f>
+        <v>306</v>
+      </c>
+      <c r="I9" s="74">
+        <f>EF_Study_Expanded!M37</f>
+        <v>7</v>
+      </c>
+      <c r="J9" s="74">
+        <f>EF_Study_Expanded!R37</f>
+        <v>763</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="74">
+        <f>EF_Study_Expanded!M44</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="74">
+        <f>EF_Study_Expanded!D51+EF_Study_Expanded!J51</f>
+        <v>116</v>
+      </c>
+      <c r="D11" s="74">
+        <f>EF_Study_Expanded!E51</f>
+        <v>32</v>
+      </c>
+      <c r="E11" s="74">
+        <f>EF_Study_Expanded!F51</f>
+        <v>7</v>
+      </c>
+      <c r="F11" s="74">
+        <f>EF_Study_Expanded!G51</f>
+        <v>3</v>
+      </c>
+      <c r="G11" s="74">
+        <f>EF_Study_Expanded!I51</f>
+        <v>18</v>
+      </c>
+      <c r="I11" s="74" t="str">
+        <f>EF_Study_Expanded!M51</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J11" s="74">
+        <f>EF_Study_Expanded!R51</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74"/>
+      <c r="K12">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="C15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>113</v>
+      </c>
+      <c r="E16">
+        <v>54</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11">
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>41</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>51</v>
+      </c>
+      <c r="I17">
+        <v>305</v>
+      </c>
+      <c r="J17">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11">
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19">
+        <v>14</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="I19">
+        <v>41</v>
+      </c>
+      <c r="J19">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20">
+        <v>481</v>
+      </c>
+      <c r="D20">
+        <v>139</v>
+      </c>
+      <c r="E20">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20">
+        <v>95</v>
+      </c>
+      <c r="H20">
+        <v>306</v>
+      </c>
+      <c r="I20">
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22">
+        <v>116</v>
+      </c>
+      <c r="D22">
+        <v>32</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>18</v>
+      </c>
+      <c r="I22" t="s">
+        <v>77</v>
+      </c>
+      <c r="J22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="K23">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="B26" s="75" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26">
+        <v>38</v>
+      </c>
+      <c r="E26">
+        <v>50</v>
+      </c>
+      <c r="G26">
+        <v>21</v>
+      </c>
+      <c r="H26">
+        <v>481</v>
+      </c>
+      <c r="J26">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="B27" s="75"/>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27">
+        <v>113</v>
+      </c>
+      <c r="E27">
+        <v>41</v>
+      </c>
+      <c r="G27">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <v>139</v>
+      </c>
+      <c r="J27">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="B28" s="75"/>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>54</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28">
+        <v>13</v>
+      </c>
+      <c r="J28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="B29" s="75"/>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>14</v>
+      </c>
+      <c r="H29" t="s">
+        <v>77</v>
+      </c>
+      <c r="J29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" s="75"/>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30">
+        <v>51</v>
+      </c>
+      <c r="G30">
+        <v>18</v>
+      </c>
+      <c r="H30">
+        <v>95</v>
+      </c>
+      <c r="J30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11">
+      <c r="B31" s="75" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11">
+      <c r="B32" s="75"/>
+      <c r="H32">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11">
+      <c r="B33" s="75"/>
+    </row>
+    <row r="34" spans="2:11">
+      <c r="B34" s="75" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11">
+      <c r="B35" s="75"/>
+      <c r="D35" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35">
+        <v>305</v>
+      </c>
+      <c r="F35">
+        <v>377</v>
+      </c>
+      <c r="G35">
+        <v>41</v>
+      </c>
+      <c r="H35">
+        <v>7</v>
+      </c>
+      <c r="I35">
+        <v>80</v>
+      </c>
+      <c r="J35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11">
+      <c r="B36" s="75"/>
+    </row>
+    <row r="38" spans="2:11">
+      <c r="D38" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" t="s">
+        <v>32</v>
+      </c>
+      <c r="H38" t="s">
+        <v>33</v>
+      </c>
+      <c r="I38" t="s">
+        <v>34</v>
+      </c>
+      <c r="J38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11">
+      <c r="B39" s="75" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39">
+        <v>38</v>
+      </c>
+      <c r="E39">
+        <v>50</v>
+      </c>
+      <c r="G39">
+        <v>21</v>
+      </c>
+      <c r="H39">
+        <v>481</v>
+      </c>
+      <c r="J39">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="B40" s="75"/>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40">
+        <v>113</v>
+      </c>
+      <c r="E40">
+        <v>41</v>
+      </c>
+      <c r="G40">
+        <v>9</v>
+      </c>
+      <c r="H40">
+        <v>139</v>
+      </c>
+      <c r="J40">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11">
+      <c r="B41" s="75"/>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41">
+        <v>54</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="G41" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41">
+        <v>13</v>
+      </c>
+      <c r="J41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11">
+      <c r="B42" s="75"/>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="G42">
+        <v>14</v>
+      </c>
+      <c r="H42" t="s">
+        <v>77</v>
+      </c>
+      <c r="J42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11">
+      <c r="B43" s="75"/>
+      <c r="C43" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43">
+        <v>51</v>
+      </c>
+      <c r="G43">
+        <v>18</v>
+      </c>
+      <c r="H43">
+        <v>95</v>
+      </c>
+      <c r="J43">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11">
+      <c r="B44" s="75"/>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>30</v>
+      </c>
+      <c r="E44">
+        <v>74</v>
+      </c>
+      <c r="G44">
+        <v>82</v>
+      </c>
+      <c r="H44">
+        <v>763</v>
+      </c>
+      <c r="J44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11">
+      <c r="B45" s="75" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="B46" s="75"/>
+      <c r="C46" t="s">
+        <v>81</v>
+      </c>
+      <c r="H46">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11">
+      <c r="B47" s="75"/>
+    </row>
+    <row r="48" spans="2:11">
+      <c r="B48" s="75" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11">
+      <c r="B49" s="75"/>
+      <c r="C49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49">
+        <v>305</v>
+      </c>
+      <c r="F49">
+        <v>377</v>
+      </c>
+      <c r="G49">
+        <v>41</v>
+      </c>
+      <c r="H49">
+        <v>7</v>
+      </c>
+      <c r="I49">
+        <v>80</v>
+      </c>
+      <c r="J49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11">
+      <c r="B50" s="75"/>
+    </row>
+    <row r="51" spans="2:11">
+      <c r="B51" s="75" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11">
+      <c r="B52" s="75"/>
+      <c r="C52" t="s">
+        <v>86</v>
+      </c>
+      <c r="K52">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11">
+      <c r="B53" s="75"/>
+    </row>
+    <row r="55" spans="2:11">
+      <c r="D55">
+        <f>SUM(D39:D44)</f>
+        <v>245</v>
+      </c>
+      <c r="E55">
+        <f t="shared" ref="E55:K55" si="0">SUM(E39:E44)</f>
+        <v>224</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="0"/>
+        <v>1491</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="0"/>
+        <v>191</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11">
+      <c r="D56">
+        <f>D55/3441</f>
+        <v>7.1200232490555071E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11">
+      <c r="D57">
+        <f>SUM(D39:K52)</f>
+        <v>3518</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>